<commit_message>
#17: Corrected power switch pin
</commit_message>
<xml_diff>
--- a/docs/PinoutTable_v1.0.0__RPi_3bp__Breadboard_v1.0.0.xlsx
+++ b/docs/PinoutTable_v1.0.0__RPi_3bp__Breadboard_v1.0.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\SW_Projects\GestureControl\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9115489-1401-4537-B4AB-D542F6AFF8A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7220270F-D355-4550-AD42-2B0F1DBFE73C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{80607C14-953B-4F4B-8B21-B95F1610CABD}"/>
   </bookViews>
@@ -57,12 +57,6 @@
     <t>Last Modified Date</t>
   </si>
   <si>
-    <t>Positive Power Rail</t>
-  </si>
-  <si>
-    <t>Red Rail</t>
-  </si>
-  <si>
     <t>Accel/Gyro/Mag</t>
   </si>
   <si>
@@ -112,6 +106,12 @@
   </si>
   <si>
     <t>Mux select lines (MCP and PIP mux selects are wired together on breadboard)</t>
+  </si>
+  <si>
+    <t>Power Regulator Circuit</t>
+  </si>
+  <si>
+    <t>Toggle Switch</t>
   </si>
 </sst>
 </file>
@@ -885,7 +885,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,13 +954,13 @@
         <v>2</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -968,10 +968,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" s="34"/>
       <c r="E6" s="30">
@@ -986,10 +986,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="D7" s="34"/>
       <c r="E7" s="30">
@@ -1010,10 +1010,10 @@
         <v>8</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H8" s="21"/>
     </row>
@@ -1022,22 +1022,22 @@
         <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="34" t="s">
         <v>15</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="34" t="s">
-        <v>17</v>
       </c>
       <c r="E9" s="30">
         <v>10</v>
       </c>
       <c r="F9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="H9" s="21"/>
     </row>
@@ -1102,13 +1102,13 @@
         <v>19</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C14" s="4">
         <v>14</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E14" s="30">
         <v>20</v>
@@ -1122,13 +1122,13 @@
         <v>21</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" s="4">
         <v>13</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E15" s="30">
         <v>22</v>
@@ -1142,13 +1142,13 @@
         <v>23</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C16" s="4">
         <v>12</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E16" s="30">
         <v>24</v>
@@ -1168,13 +1168,13 @@
         <v>26</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G17" s="6">
         <v>15</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1244,13 +1244,13 @@
         <v>36</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G22" s="6">
         <v>14</v>
       </c>
       <c r="H22" s="21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1264,13 +1264,13 @@
         <v>38</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G23" s="6">
         <v>15</v>
       </c>
       <c r="H23" s="21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1284,13 +1284,13 @@
         <v>40</v>
       </c>
       <c r="F24" s="26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G24" s="25">
         <v>16</v>
       </c>
       <c r="H24" s="27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>